<commit_message>
adding the test environment column
</commit_message>
<xml_diff>
--- a/Sharlen Website/Check list for Sharlen web site .xlsx
+++ b/Sharlen Website/Check list for Sharlen web site .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahm0\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\TestingProgects\Sharlen Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A68203-7AEB-4CD3-AE25-2AFAC3CD1E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EC1D1E-22C8-49C5-AAA1-2E878E1E3F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="210">
   <si>
     <t xml:space="preserve">TC_ID </t>
   </si>
@@ -929,6 +929,12 @@
   </si>
   <si>
     <t xml:space="preserve">Author : Mahmoud Mohamed Hamed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test environment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsfot Edge </t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1133,12 +1139,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1148,9 +1148,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1158,9 +1155,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1195,6 +1189,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1487,958 +1497,1071 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I193"/>
+  <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="6" width="30.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" customWidth="1"/>
+    <col min="4" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="J5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="H10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="J10" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="H11" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="24"/>
+      <c r="J11" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="H12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="I12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="8" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="H13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="I13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="8" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="I14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="8" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="H15" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="I15" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="J15" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="8" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="H16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="H17" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="I17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="J17" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="H18" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="I18" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I19" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="H20" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="I20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="J20" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="24"/>
+      <c r="D21" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="H21" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="I21" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="J21" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="8" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="H22" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="I22" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="8" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="H23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="I23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="8" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="24"/>
+      <c r="J24" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="H25" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="H26" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="I26" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="J26" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="8" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="H27" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="I27" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="8" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="H28" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="I28" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="J28" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="8" t="s">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="H29" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="I29" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="J29" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="8" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="H30" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="I30" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="J30" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="H31" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="I31" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="J31" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="8" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="H32" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="I32" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="J32" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="8" t="s">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="H33" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="J33" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="H34" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="I34" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="J34" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="8" t="s">
+      <c r="C35" s="24"/>
+      <c r="D35" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="E35" s="6"/>
+      <c r="F35" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="H35" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="I35" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="J35" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12" t="s">
+      <c r="C36" s="24"/>
+      <c r="D36" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12" t="s">
+      <c r="E36" s="9"/>
+      <c r="F36" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="H36" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="I36" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="J36" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:10" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="24"/>
+      <c r="D37" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G37" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="H37" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="I37" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="J37" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2448,8 +2571,9 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2459,8 +2583,9 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2470,8 +2595,9 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2481,8 +2607,9 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2492,8 +2619,9 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2503,8 +2631,9 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2514,8 +2643,9 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2525,8 +2655,9 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2536,8 +2667,9 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2547,8 +2679,9 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2558,8 +2691,9 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2569,8 +2703,9 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2580,8 +2715,9 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2591,8 +2727,9 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2602,8 +2739,9 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2613,8 +2751,9 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2624,8 +2763,9 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2635,8 +2775,9 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2646,8 +2787,9 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2657,8 +2799,9 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2668,8 +2811,9 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2679,8 +2823,9 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2690,8 +2835,9 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2701,8 +2847,9 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2712,8 +2859,9 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2723,8 +2871,9 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2734,8 +2883,9 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2745,8 +2895,9 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2756,8 +2907,9 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2767,8 +2919,9 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2778,8 +2931,9 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2789,8 +2943,9 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2800,8 +2955,9 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2811,8 +2967,9 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2822,8 +2979,9 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2833,8 +2991,9 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2843,8 +3002,9 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2853,8 +3013,9 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2863,8 +3024,9 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2873,8 +3035,9 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2883,8 +3046,9 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2893,8 +3057,9 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2903,8 +3068,9 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2913,8 +3079,9 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2923,8 +3090,9 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2933,8 +3101,9 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2943,8 +3112,9 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2953,8 +3123,9 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2963,8 +3134,9 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2973,8 +3145,9 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2983,8 +3156,9 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2993,8 +3167,9 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3003,8 +3178,9 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3013,8 +3189,9 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3023,8 +3200,9 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3033,8 +3211,9 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3043,8 +3222,9 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3053,8 +3233,9 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3063,8 +3244,9 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3073,8 +3255,9 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3083,8 +3266,9 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3093,8 +3277,9 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3103,8 +3288,9 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3113,8 +3299,9 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3123,8 +3310,9 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3133,8 +3321,9 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3143,8 +3332,9 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3153,8 +3343,9 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3163,8 +3354,9 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3173,8 +3365,9 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3183,8 +3376,9 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3193,8 +3387,9 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3203,8 +3398,9 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3213,8 +3409,9 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3223,8 +3420,9 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3233,8 +3431,9 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="1"/>
+    </row>
+    <row r="114" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3243,8 +3442,9 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3253,8 +3453,9 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3263,8 +3464,9 @@
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3273,8 +3475,9 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3283,8 +3486,9 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3293,8 +3497,9 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3303,8 +3508,9 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3313,8 +3519,9 @@
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3323,8 +3530,9 @@
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3333,8 +3541,9 @@
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3343,8 +3552,9 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3353,8 +3563,9 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3363,8 +3574,9 @@
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3373,8 +3585,9 @@
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3383,8 +3596,9 @@
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="1"/>
+    </row>
+    <row r="129" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3393,8 +3607,9 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="1"/>
+    </row>
+    <row r="130" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3403,8 +3618,9 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3413,8 +3629,9 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3423,8 +3640,9 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3433,8 +3651,9 @@
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3443,8 +3662,9 @@
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3453,8 +3673,9 @@
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="1"/>
+    </row>
+    <row r="136" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3463,8 +3684,9 @@
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="1"/>
+    </row>
+    <row r="137" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3473,8 +3695,9 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="1"/>
+    </row>
+    <row r="138" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3483,8 +3706,9 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="1"/>
+    </row>
+    <row r="139" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3493,8 +3717,9 @@
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="1"/>
+    </row>
+    <row r="140" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3503,8 +3728,9 @@
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="1"/>
+    </row>
+    <row r="141" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3513,8 +3739,9 @@
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="1"/>
+    </row>
+    <row r="142" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3523,8 +3750,9 @@
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="1"/>
+    </row>
+    <row r="143" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3533,8 +3761,9 @@
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="1"/>
+    </row>
+    <row r="144" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3543,8 +3772,9 @@
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="1"/>
+    </row>
+    <row r="145" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3553,8 +3783,9 @@
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="1"/>
+    </row>
+    <row r="146" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3563,8 +3794,9 @@
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="1"/>
+    </row>
+    <row r="147" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3573,8 +3805,9 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="1"/>
+    </row>
+    <row r="148" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3583,8 +3816,9 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="1"/>
+    </row>
+    <row r="149" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3593,8 +3827,9 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="1"/>
+    </row>
+    <row r="150" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3603,8 +3838,9 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="1"/>
+    </row>
+    <row r="151" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3613,8 +3849,9 @@
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="1"/>
+    </row>
+    <row r="152" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3623,8 +3860,9 @@
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="1"/>
+    </row>
+    <row r="153" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3633,8 +3871,9 @@
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="1"/>
+    </row>
+    <row r="154" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3643,8 +3882,9 @@
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="1"/>
+    </row>
+    <row r="155" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3653,8 +3893,9 @@
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="1"/>
+    </row>
+    <row r="156" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3663,8 +3904,9 @@
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="1"/>
+    </row>
+    <row r="157" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3673,8 +3915,9 @@
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="1"/>
+    </row>
+    <row r="158" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3683,8 +3926,9 @@
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" s="1"/>
+    </row>
+    <row r="159" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3693,8 +3937,9 @@
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="1"/>
+    </row>
+    <row r="160" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3703,8 +3948,9 @@
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" s="1"/>
+    </row>
+    <row r="161" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3713,8 +3959,9 @@
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" s="1"/>
+    </row>
+    <row r="162" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3723,8 +3970,9 @@
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" s="1"/>
+    </row>
+    <row r="163" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3733,8 +3981,9 @@
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" s="1"/>
+    </row>
+    <row r="164" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3743,8 +3992,9 @@
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" s="1"/>
+    </row>
+    <row r="165" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3753,8 +4003,9 @@
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" s="1"/>
+    </row>
+    <row r="166" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3763,8 +4014,9 @@
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" s="1"/>
+    </row>
+    <row r="167" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3773,8 +4025,9 @@
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" s="1"/>
+    </row>
+    <row r="168" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3783,8 +4036,9 @@
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" s="1"/>
+    </row>
+    <row r="169" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3793,8 +4047,9 @@
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" s="1"/>
+    </row>
+    <row r="170" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3803,8 +4058,9 @@
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" s="1"/>
+    </row>
+    <row r="171" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3813,8 +4069,9 @@
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" s="1"/>
+    </row>
+    <row r="172" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3823,8 +4080,9 @@
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" s="1"/>
+    </row>
+    <row r="173" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3833,8 +4091,9 @@
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" s="1"/>
+    </row>
+    <row r="174" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3843,8 +4102,9 @@
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" s="1"/>
+    </row>
+    <row r="175" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3853,8 +4113,9 @@
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" s="1"/>
+    </row>
+    <row r="176" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3863,8 +4124,9 @@
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" s="1"/>
+    </row>
+    <row r="177" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3873,8 +4135,9 @@
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="1"/>
+    </row>
+    <row r="178" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3883,8 +4146,9 @@
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" s="1"/>
+    </row>
+    <row r="179" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3893,8 +4157,9 @@
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" s="1"/>
+    </row>
+    <row r="180" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3903,8 +4168,9 @@
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" s="1"/>
+    </row>
+    <row r="181" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3913,8 +4179,9 @@
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" s="1"/>
+    </row>
+    <row r="182" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3923,8 +4190,9 @@
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" s="1"/>
+    </row>
+    <row r="183" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3933,8 +4201,9 @@
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" s="1"/>
+    </row>
+    <row r="184" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3943,8 +4212,9 @@
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I184" s="1"/>
+    </row>
+    <row r="185" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3953,8 +4223,9 @@
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" s="1"/>
+    </row>
+    <row r="186" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3963,8 +4234,9 @@
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I186" s="1"/>
+    </row>
+    <row r="187" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3973,8 +4245,9 @@
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" s="1"/>
+    </row>
+    <row r="188" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3983,8 +4256,9 @@
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" s="1"/>
+    </row>
+    <row r="189" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3993,8 +4267,9 @@
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" s="1"/>
+    </row>
+    <row r="190" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4003,8 +4278,9 @@
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" s="1"/>
+    </row>
+    <row r="191" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4013,8 +4289,9 @@
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" s="1"/>
+    </row>
+    <row r="192" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4023,8 +4300,9 @@
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I192" s="1"/>
+    </row>
+    <row r="193" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4033,31 +4311,32 @@
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
+      <c r="I193" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C17:C24"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C8:C11"/>
-    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4081,19 +4360,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="27"/>
+      <c r="D1" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4336,20 +4615,20 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>